<commit_message>
add 0x10F8 and new SDOs
</commit_message>
<xml_diff>
--- a/lib/soes-esi/lan9252_spi.xlsx
+++ b/lib/soes-esi/lan9252_spi.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\my-projects\work\crc-inc\workspace\soes-stm32f3\lib\soes-esi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4D5A04A-A109-461A-93A2-50CF30D0C9F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3B23771-0FF5-479D-99F3-28DEDD61B3B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="Profile" sheetId="11" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Profile!$B$10:$P$201</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Profile!$B$1:$P$202</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Profile!$B$10:$P$210</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Profile!$B$1:$P$211</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="105">
   <si>
     <t>Index</t>
   </si>
@@ -449,6 +449,24 @@
   </si>
   <si>
     <t>RTD 50/60 Hz Filter</t>
+  </si>
+  <si>
+    <t>0x8002</t>
+  </si>
+  <si>
+    <t>0x8003</t>
+  </si>
+  <si>
+    <t>RTD High Threshold</t>
+  </si>
+  <si>
+    <t>RTD Low Threshold</t>
+  </si>
+  <si>
+    <t>0x8004</t>
+  </si>
+  <si>
+    <t>IMU Full Scale</t>
   </si>
 </sst>
 </file>
@@ -869,11 +887,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:T205"/>
+  <dimension ref="B1:T214"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D84" sqref="D84"/>
+      <pane ySplit="10" topLeftCell="A167" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J175" sqref="J175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -4837,7 +4855,7 @@
       <c r="D191" s="8"/>
       <c r="E191" s="10"/>
       <c r="F191" s="10" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="G191" s="10"/>
       <c r="H191" s="10"/>
@@ -4854,7 +4872,7 @@
         <v>1</v>
       </c>
       <c r="E192" s="10" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="F192" s="10"/>
       <c r="G192" s="10" t="s">
@@ -4870,38 +4888,54 @@
       <c r="P192"/>
     </row>
     <row r="193" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="D193" s="8"/>
+      <c r="E193" s="10"/>
+      <c r="F193" s="10"/>
+      <c r="G193" s="10"/>
+      <c r="H193" s="10"/>
+      <c r="I193" s="10"/>
       <c r="N193"/>
       <c r="O193"/>
       <c r="P193"/>
     </row>
-    <row r="194" spans="2:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B194" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C194" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D194" s="11"/>
-      <c r="E194" s="11"/>
-      <c r="F194" s="11"/>
-      <c r="G194" s="11"/>
-      <c r="H194" s="11"/>
-      <c r="I194" s="11"/>
-      <c r="J194" s="11"/>
-      <c r="K194" s="11"/>
-      <c r="L194" s="11"/>
-      <c r="M194" s="11"/>
-      <c r="N194" s="11"/>
-      <c r="O194" s="11"/>
-      <c r="P194" s="11"/>
+    <row r="194" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B194" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C194" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D194" s="8"/>
+      <c r="E194" s="10"/>
+      <c r="F194" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="G194" s="10"/>
+      <c r="H194" s="10"/>
+      <c r="I194" s="10"/>
+      <c r="L194" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="N194"/>
+      <c r="O194"/>
+      <c r="P194"/>
     </row>
     <row r="195" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D195" s="8"/>
-      <c r="E195" s="10"/>
+      <c r="D195" s="8">
+        <v>1</v>
+      </c>
+      <c r="E195" s="10" t="s">
+        <v>47</v>
+      </c>
       <c r="F195" s="10"/>
-      <c r="G195" s="10"/>
+      <c r="G195" s="10" t="s">
+        <v>41</v>
+      </c>
       <c r="H195" s="10"/>
       <c r="I195" s="10"/>
+      <c r="L195" s="2" t="s">
+        <v>60</v>
+      </c>
       <c r="N195"/>
       <c r="O195"/>
       <c r="P195"/>
@@ -4917,34 +4951,44 @@
       <c r="O196"/>
       <c r="P196"/>
     </row>
-    <row r="197" spans="2:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B197" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C197" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D197" s="11"/>
-      <c r="E197" s="11"/>
-      <c r="F197" s="11"/>
-      <c r="G197" s="11"/>
-      <c r="H197" s="11"/>
-      <c r="I197" s="11"/>
-      <c r="J197" s="11"/>
-      <c r="K197" s="11"/>
-      <c r="L197" s="11"/>
-      <c r="M197" s="11"/>
-      <c r="N197" s="11"/>
-      <c r="O197" s="11"/>
-      <c r="P197" s="11"/>
+    <row r="197" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B197" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C197" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D197" s="8"/>
+      <c r="E197" s="10"/>
+      <c r="F197" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="G197" s="10"/>
+      <c r="H197" s="10"/>
+      <c r="I197" s="10"/>
+      <c r="L197" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="N197"/>
+      <c r="O197"/>
+      <c r="P197"/>
     </row>
     <row r="198" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D198" s="8"/>
-      <c r="E198" s="10"/>
+      <c r="D198" s="8">
+        <v>1</v>
+      </c>
+      <c r="E198" s="10" t="s">
+        <v>59</v>
+      </c>
       <c r="F198" s="10"/>
-      <c r="G198" s="10"/>
+      <c r="G198" s="10" t="s">
+        <v>41</v>
+      </c>
       <c r="H198" s="10"/>
       <c r="I198" s="10"/>
+      <c r="L198" s="2" t="s">
+        <v>60</v>
+      </c>
       <c r="N198"/>
       <c r="O198"/>
       <c r="P198"/>
@@ -4960,128 +5004,267 @@
       <c r="O199"/>
       <c r="P199"/>
     </row>
-    <row r="200" spans="2:16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B200" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="C200" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="D200" s="13"/>
-      <c r="E200" s="13"/>
-      <c r="F200" s="13"/>
-      <c r="G200" s="13"/>
-      <c r="H200" s="13"/>
-      <c r="I200" s="13"/>
-      <c r="J200" s="13"/>
-      <c r="K200" s="13"/>
-      <c r="L200" s="13"/>
-      <c r="M200" s="13"/>
-      <c r="N200" s="13"/>
-      <c r="O200" s="11"/>
-      <c r="P200" s="11"/>
+    <row r="200" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B200" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C200" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D200" s="8"/>
+      <c r="E200" s="10"/>
+      <c r="F200" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="G200" s="10"/>
+      <c r="H200" s="10"/>
+      <c r="I200" s="10"/>
+      <c r="L200" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="N200"/>
+      <c r="O200"/>
+      <c r="P200"/>
     </row>
     <row r="201" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B201"/>
-      <c r="C201"/>
-      <c r="D201"/>
-      <c r="E201"/>
-      <c r="F201"/>
-      <c r="G201"/>
-      <c r="H201"/>
-      <c r="I201"/>
-      <c r="J201"/>
-      <c r="K201"/>
-      <c r="L201"/>
-      <c r="M201"/>
+      <c r="D201" s="8">
+        <v>1</v>
+      </c>
+      <c r="E201" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="F201" s="10"/>
+      <c r="G201" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="H201" s="10"/>
+      <c r="I201" s="10"/>
+      <c r="L201" s="2" t="s">
+        <v>60</v>
+      </c>
       <c r="N201"/>
       <c r="O201"/>
       <c r="P201"/>
     </row>
     <row r="202" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B202"/>
-      <c r="C202"/>
-      <c r="D202"/>
-      <c r="E202"/>
-      <c r="F202"/>
-      <c r="G202"/>
-      <c r="H202"/>
-      <c r="I202"/>
-      <c r="J202"/>
-      <c r="K202"/>
-      <c r="L202"/>
-      <c r="M202"/>
-      <c r="N202" s="14"/>
+      <c r="D202" s="8"/>
+      <c r="E202" s="10"/>
+      <c r="F202" s="10"/>
+      <c r="G202" s="10"/>
+      <c r="H202" s="10"/>
+      <c r="I202" s="10"/>
+      <c r="N202"/>
       <c r="O202"/>
       <c r="P202"/>
     </row>
-    <row r="203" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B203"/>
-      <c r="C203"/>
-      <c r="D203"/>
-      <c r="E203"/>
-      <c r="F203"/>
-      <c r="G203"/>
-      <c r="H203"/>
-      <c r="I203"/>
-      <c r="J203"/>
-      <c r="K203"/>
-      <c r="L203"/>
-      <c r="M203"/>
-      <c r="N203"/>
+    <row r="203" spans="2:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B203" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C203" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D203" s="11"/>
+      <c r="E203" s="11"/>
+      <c r="F203" s="11"/>
+      <c r="G203" s="11"/>
+      <c r="H203" s="11"/>
+      <c r="I203" s="11"/>
+      <c r="J203" s="11"/>
+      <c r="K203" s="11"/>
+      <c r="L203" s="11"/>
+      <c r="M203" s="11"/>
+      <c r="N203" s="11"/>
+      <c r="O203" s="11"/>
+      <c r="P203" s="11"/>
     </row>
     <row r="204" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B204"/>
-      <c r="C204"/>
-      <c r="D204"/>
-      <c r="E204"/>
-      <c r="F204"/>
-      <c r="G204"/>
-      <c r="H204"/>
-      <c r="I204"/>
-      <c r="J204"/>
-      <c r="K204"/>
-      <c r="L204"/>
-      <c r="M204"/>
-      <c r="N204" s="14"/>
+      <c r="D204" s="8"/>
+      <c r="E204" s="10"/>
+      <c r="F204" s="10"/>
+      <c r="G204" s="10"/>
+      <c r="H204" s="10"/>
+      <c r="I204" s="10"/>
+      <c r="N204"/>
+      <c r="O204"/>
+      <c r="P204"/>
     </row>
     <row r="205" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B205"/>
-      <c r="C205"/>
-      <c r="D205"/>
-      <c r="E205"/>
-      <c r="F205"/>
-      <c r="G205"/>
-      <c r="H205"/>
-      <c r="I205"/>
-      <c r="J205"/>
-      <c r="K205"/>
-      <c r="L205"/>
-      <c r="M205"/>
+      <c r="D205" s="8"/>
+      <c r="E205" s="10"/>
+      <c r="F205" s="10"/>
+      <c r="G205" s="10"/>
+      <c r="H205" s="10"/>
+      <c r="I205" s="10"/>
       <c r="N205"/>
+      <c r="O205"/>
+      <c r="P205"/>
+    </row>
+    <row r="206" spans="2:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B206" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C206" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D206" s="11"/>
+      <c r="E206" s="11"/>
+      <c r="F206" s="11"/>
+      <c r="G206" s="11"/>
+      <c r="H206" s="11"/>
+      <c r="I206" s="11"/>
+      <c r="J206" s="11"/>
+      <c r="K206" s="11"/>
+      <c r="L206" s="11"/>
+      <c r="M206" s="11"/>
+      <c r="N206" s="11"/>
+      <c r="O206" s="11"/>
+      <c r="P206" s="11"/>
+    </row>
+    <row r="207" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="D207" s="8"/>
+      <c r="E207" s="10"/>
+      <c r="F207" s="10"/>
+      <c r="G207" s="10"/>
+      <c r="H207" s="10"/>
+      <c r="I207" s="10"/>
+      <c r="N207"/>
+      <c r="O207"/>
+      <c r="P207"/>
+    </row>
+    <row r="208" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="D208" s="8"/>
+      <c r="E208" s="10"/>
+      <c r="F208" s="10"/>
+      <c r="G208" s="10"/>
+      <c r="H208" s="10"/>
+      <c r="I208" s="10"/>
+      <c r="N208"/>
+      <c r="O208"/>
+      <c r="P208"/>
+    </row>
+    <row r="209" spans="2:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B209" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C209" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D209" s="13"/>
+      <c r="E209" s="13"/>
+      <c r="F209" s="13"/>
+      <c r="G209" s="13"/>
+      <c r="H209" s="13"/>
+      <c r="I209" s="13"/>
+      <c r="J209" s="13"/>
+      <c r="K209" s="13"/>
+      <c r="L209" s="13"/>
+      <c r="M209" s="13"/>
+      <c r="N209" s="13"/>
+      <c r="O209" s="11"/>
+      <c r="P209" s="11"/>
+    </row>
+    <row r="210" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B210"/>
+      <c r="C210"/>
+      <c r="D210"/>
+      <c r="E210"/>
+      <c r="F210"/>
+      <c r="G210"/>
+      <c r="H210"/>
+      <c r="I210"/>
+      <c r="J210"/>
+      <c r="K210"/>
+      <c r="L210"/>
+      <c r="M210"/>
+      <c r="N210"/>
+      <c r="O210"/>
+      <c r="P210"/>
+    </row>
+    <row r="211" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B211"/>
+      <c r="C211"/>
+      <c r="D211"/>
+      <c r="E211"/>
+      <c r="F211"/>
+      <c r="G211"/>
+      <c r="H211"/>
+      <c r="I211"/>
+      <c r="J211"/>
+      <c r="K211"/>
+      <c r="L211"/>
+      <c r="M211"/>
+      <c r="N211" s="14"/>
+      <c r="O211"/>
+      <c r="P211"/>
+    </row>
+    <row r="212" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B212"/>
+      <c r="C212"/>
+      <c r="D212"/>
+      <c r="E212"/>
+      <c r="F212"/>
+      <c r="G212"/>
+      <c r="H212"/>
+      <c r="I212"/>
+      <c r="J212"/>
+      <c r="K212"/>
+      <c r="L212"/>
+      <c r="M212"/>
+      <c r="N212"/>
+    </row>
+    <row r="213" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B213"/>
+      <c r="C213"/>
+      <c r="D213"/>
+      <c r="E213"/>
+      <c r="F213"/>
+      <c r="G213"/>
+      <c r="H213"/>
+      <c r="I213"/>
+      <c r="J213"/>
+      <c r="K213"/>
+      <c r="L213"/>
+      <c r="M213"/>
+      <c r="N213" s="14"/>
+    </row>
+    <row r="214" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B214"/>
+      <c r="C214"/>
+      <c r="D214"/>
+      <c r="E214"/>
+      <c r="F214"/>
+      <c r="G214"/>
+      <c r="H214"/>
+      <c r="I214"/>
+      <c r="J214"/>
+      <c r="K214"/>
+      <c r="L214"/>
+      <c r="M214"/>
+      <c r="N214"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatRows="0" insertRows="0" insertHyperlinks="0" deleteRows="0" sort="0" autoFilter="0"/>
-  <autoFilter ref="B10:P201" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="B10:P210" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="1">
     <mergeCell ref="F1:P6"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C213:C1052" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C222:C1061" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"VARIABLE,ARRAY,RECORD"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M15:M16 M18:M19 M21:M22 M27:M28 M30:M31 M33:M34 M12:M13 M195:M196 M198:M201 M24:M25 M153:M186 M188:M193 M36:M151" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M15:M16 M18:M19 M21:M22 M27:M28 M30:M31 M33:M34 M12:M13 M204:M205 M207:M210 M24:M25 M153:M186 M188:M202 M36:M151" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"rx,tx"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Object Code value" error="The Object code value shall be:_x000a_VARIABLE_x000a_RECORD_x000a_ARRAY" sqref="C12:C13 C15:C16 C18:C19 C21:C22 C27:C28 C30:C31 C33:C34 C153:C186 C195:C196 C198:C212 C24:C25 C36:C151 C188:C192" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Object Code value" error="The Object code value shall be:_x000a_VARIABLE_x000a_RECORD_x000a_ARRAY" sqref="C12:C13 C15:C16 C18:C19 C21:C22 C27:C28 C30:C31 C33:C34 C153:C186 C204:C205 C207:C221 C24:C25 C36:C151 C188:C202" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"VARIABLE,ARRAY,RECORD"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" sqref="C11 C14 C17 C20 C23 C26 C29 C32 C35 C152 C187 C194 C197" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Category" error="The value for the entry category shall be _x000a_M : (mandatory)_x000a_O : (optional) _x000a_C : (conditional)" sqref="J12:J13 J15:J16 J18:J19 J21:J22 J27:J28 J30:J31 J33:J34 J153:J186 J195:J196 J198:J212 J24:J25 J36:J151 J188:J192" xr:uid="{00000000-0002-0000-0000-000004000000}">
+    <dataValidation allowBlank="1" showInputMessage="1" sqref="C11 C14 C17 C20 C23 C26 C29 C32 C35 C152 C187 C203 C206" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Category" error="The value for the entry category shall be _x000a_M : (mandatory)_x000a_O : (optional) _x000a_C : (conditional)" sqref="J12:J13 J15:J16 J18:J19 J21:J22 J27:J28 J30:J31 J33:J34 J153:J186 J204:J205 J207:J221 J24:J25 J36:J151 J188:J202" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>"M,O,C"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Backup/Setting Flag" error="The entry flag shall be_x000a_B : (Backup)_x000a_S : (Setting)" sqref="K12:K13 K15:K16 K18:K19 K21:K22 K27:K28 K30:K31 K33:K34 K153:K186 K195:K196 K198:K212 K24:K25 K36:K151 K188:K192" xr:uid="{00000000-0002-0000-0000-000005000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Backup/Setting Flag" error="The entry flag shall be_x000a_B : (Backup)_x000a_S : (Setting)" sqref="K12:K13 K15:K16 K18:K19 K21:K22 K27:K28 K30:K31 K33:K34 K153:K186 K204:K205 K207:K221 K24:K25 K36:K151 K188:K202" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>"B,S"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5094,6 +5277,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100ED35F0256D409E42987BF98036DA9989" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="61ea75deb4a032f98cafe45aa38f3ba3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="ab83d208-b7b8-4829-a129-d03539c0c0d7" xmlns:ns4="ef89b0e5-7345-4605-9a1c-4acb13fb8c8a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3580dc75d458420bc34e35ba09e33716" ns3:_="" ns4:_="">
     <xsd:import namespace="ab83d208-b7b8-4829-a129-d03539c0c0d7"/>
@@ -5308,15 +5500,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -5324,6 +5507,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AFB03729-4752-40CC-AACD-E363FA2FB05F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF0CCFE4-F70B-4F14-929D-A6D65641CA19}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5338,14 +5529,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AFB03729-4752-40CC-AACD-E363FA2FB05F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>